<commit_message>
Replace xlsx test files
</commit_message>
<xml_diff>
--- a/packages/central-server/__tests__/importers/programs-charting-complex-core-hidden-question-invalid.xlsx
+++ b/packages/central-server/__tests__/importers/programs-charting-complex-core-hidden-question-invalid.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
   <si>
     <t>programName</t>
   </si>
@@ -126,9 +126,6 @@
     <t>visibilityStatus</t>
   </si>
   <si>
-    <t>testchartcorecode0</t>
-  </si>
-  <si>
     <t>ComplexChartInstanceName</t>
   </si>
   <si>
@@ -138,18 +135,12 @@
     <t>historical</t>
   </si>
   <si>
-    <t>testchartcorecode1</t>
-  </si>
-  <si>
     <t>ComplexChartDate</t>
   </si>
   <si>
     <t>Date of onset</t>
   </si>
   <si>
-    <t>testchartcorecode2</t>
-  </si>
-  <si>
     <t>ComplexChartType</t>
   </si>
   <si>
@@ -162,16 +153,13 @@
     <t>current</t>
   </si>
   <si>
-    <t>testchartcorecode3</t>
-  </si>
-  <si>
     <t>ComplexChartSubtype</t>
   </si>
   <si>
     <t>Sub type</t>
   </si>
   <si>
-    <t>testchartcode0</t>
+    <t>PatientChartingDate</t>
   </si>
   <si>
     <t>DateTime</t>
@@ -472,7 +460,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.5"/>
+    <col customWidth="1" min="1" max="1" width="23.63"/>
     <col customWidth="1" min="2" max="2" width="19.0"/>
     <col customWidth="1" min="3" max="3" width="21.63"/>
     <col customWidth="1" min="4" max="4" width="16.63"/>
@@ -1641,70 +1629,70 @@
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>
@@ -2717,7 +2705,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.88"/>
+    <col customWidth="1" min="1" max="1" width="19.13"/>
     <col customWidth="1" min="2" max="2" width="12.63"/>
     <col customWidth="1" min="3" max="3" width="16.38"/>
     <col customWidth="1" min="4" max="4" width="16.63"/>
@@ -2781,62 +2769,62 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>52</v>
+      <c r="A2" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
feat(desktopCharting): SAV-700: Update charts importer (#6955)
* Ensure ID of charting date recorded program data element is constant

* Ensure ID of all complex chart core questions is constant

* This should be lowercase

* Simplify error message because its pretty redundant with stat info

* Update test cases

* Finalize tests update

* Replace xlsx test files

* Use subtype lowercase (complete cleanup is being done in another PR)

* Fix typo

Co-authored-by: Rohan Port <59544282+rohan-bes@users.noreply.github.com>

* Move to constants

Co-authored-by: Rohan Port <59544282+rohan-bes@users.noreply.github.com>

---------

Co-authored-by: Rohan Port <59544282+rohan-bes@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/packages/central-server/__tests__/importers/programs-charting-complex-core-hidden-question-invalid.xlsx
+++ b/packages/central-server/__tests__/importers/programs-charting-complex-core-hidden-question-invalid.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
   <si>
     <t>programName</t>
   </si>
@@ -126,9 +126,6 @@
     <t>visibilityStatus</t>
   </si>
   <si>
-    <t>testchartcorecode0</t>
-  </si>
-  <si>
     <t>ComplexChartInstanceName</t>
   </si>
   <si>
@@ -138,18 +135,12 @@
     <t>historical</t>
   </si>
   <si>
-    <t>testchartcorecode1</t>
-  </si>
-  <si>
     <t>ComplexChartDate</t>
   </si>
   <si>
     <t>Date of onset</t>
   </si>
   <si>
-    <t>testchartcorecode2</t>
-  </si>
-  <si>
     <t>ComplexChartType</t>
   </si>
   <si>
@@ -162,16 +153,13 @@
     <t>current</t>
   </si>
   <si>
-    <t>testchartcorecode3</t>
-  </si>
-  <si>
     <t>ComplexChartSubtype</t>
   </si>
   <si>
     <t>Sub type</t>
   </si>
   <si>
-    <t>testchartcode0</t>
+    <t>PatientChartingDate</t>
   </si>
   <si>
     <t>DateTime</t>
@@ -472,7 +460,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.5"/>
+    <col customWidth="1" min="1" max="1" width="23.63"/>
     <col customWidth="1" min="2" max="2" width="19.0"/>
     <col customWidth="1" min="3" max="3" width="21.63"/>
     <col customWidth="1" min="4" max="4" width="16.63"/>
@@ -1641,70 +1629,70 @@
         <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>
@@ -2717,7 +2705,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.88"/>
+    <col customWidth="1" min="1" max="1" width="19.13"/>
     <col customWidth="1" min="2" max="2" width="12.63"/>
     <col customWidth="1" min="3" max="3" width="16.38"/>
     <col customWidth="1" min="4" max="4" width="16.63"/>
@@ -2781,62 +2769,62 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>52</v>
+      <c r="A2" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1"/>

</xml_diff>